<commit_message>
Sprint - rotas, controller, view
</commit_message>
<xml_diff>
--- a/_project/Requisitos fornecidos pelo cliente/Agile_Scrum_Modelo_v3.xlsx
+++ b/_project/Requisitos fornecidos pelo cliente/Agile_Scrum_Modelo_v3.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD65C97-D7E9-44CC-9C00-86056AB62DD2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102D6CDC-30DA-4ADB-8BB3-FB0770611E7A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projeto" sheetId="2" r:id="rId1"/>
@@ -1719,47 +1719,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1788,11 +1749,50 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2140,7 +2140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B8" sqref="B8:B11"/>
     </sheetView>
   </sheetViews>
@@ -2944,18 +2944,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="131" t="s">
+      <c r="A1" s="118" t="s">
         <v>207</v>
       </c>
-      <c r="B1" s="132"/>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132"/>
-      <c r="I1" s="132"/>
-      <c r="J1" s="133"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="119"/>
+      <c r="J1" s="120"/>
     </row>
     <row r="2" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="41"/>
@@ -3025,30 +3025,30 @@
       <c r="J5" s="45"/>
     </row>
     <row r="6" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="134"/>
-      <c r="B6" s="135"/>
-      <c r="C6" s="135"/>
-      <c r="D6" s="135"/>
-      <c r="E6" s="135"/>
-      <c r="F6" s="135"/>
-      <c r="G6" s="135"/>
-      <c r="H6" s="135"/>
-      <c r="I6" s="135"/>
-      <c r="J6" s="136"/>
+      <c r="A6" s="121"/>
+      <c r="B6" s="122"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="122"/>
+      <c r="H6" s="122"/>
+      <c r="I6" s="122"/>
+      <c r="J6" s="123"/>
     </row>
     <row r="7" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="131" t="s">
+      <c r="A7" s="118" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="132"/>
-      <c r="C7" s="132"/>
-      <c r="D7" s="132"/>
-      <c r="E7" s="132"/>
-      <c r="F7" s="132"/>
-      <c r="G7" s="132"/>
-      <c r="H7" s="132"/>
-      <c r="I7" s="132"/>
-      <c r="J7" s="133"/>
+      <c r="B7" s="119"/>
+      <c r="C7" s="119"/>
+      <c r="D7" s="119"/>
+      <c r="E7" s="119"/>
+      <c r="F7" s="119"/>
+      <c r="G7" s="119"/>
+      <c r="H7" s="119"/>
+      <c r="I7" s="119"/>
+      <c r="J7" s="120"/>
     </row>
     <row r="8" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="38" t="s">
@@ -3083,14 +3083,14 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="129" t="s">
+      <c r="A9" s="116" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="137">
+      <c r="B9" s="124">
         <f>funcionalidades!D8</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="C9" s="139" t="str">
+      <c r="C9" s="128" t="str">
         <f>funcionalidades!E8</f>
         <v>Elaborar uma página de apresentação da empresa</v>
       </c>
@@ -3105,15 +3105,15 @@
       <c r="H9" s="33">
         <v>1</v>
       </c>
-      <c r="I9" s="137"/>
-      <c r="J9" s="138" t="s">
+      <c r="I9" s="124"/>
+      <c r="J9" s="127" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="130"/>
-      <c r="B10" s="118"/>
-      <c r="C10" s="125"/>
+      <c r="A10" s="117"/>
+      <c r="B10" s="125"/>
+      <c r="C10" s="129"/>
       <c r="D10" s="17" t="s">
         <v>71</v>
       </c>
@@ -3125,13 +3125,13 @@
       <c r="H10" s="10">
         <v>2</v>
       </c>
-      <c r="I10" s="118"/>
+      <c r="I10" s="125"/>
       <c r="J10" s="114"/>
     </row>
     <row r="11" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="130"/>
-      <c r="B11" s="118"/>
-      <c r="C11" s="125"/>
+      <c r="A11" s="117"/>
+      <c r="B11" s="125"/>
+      <c r="C11" s="129"/>
       <c r="D11" s="17" t="s">
         <v>72</v>
       </c>
@@ -3143,13 +3143,13 @@
       <c r="H11" s="10">
         <v>3</v>
       </c>
-      <c r="I11" s="118"/>
+      <c r="I11" s="125"/>
       <c r="J11" s="114"/>
     </row>
     <row r="12" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="130"/>
-      <c r="B12" s="118"/>
-      <c r="C12" s="125"/>
+      <c r="A12" s="117"/>
+      <c r="B12" s="125"/>
+      <c r="C12" s="129"/>
       <c r="D12" s="17" t="s">
         <v>73</v>
       </c>
@@ -3161,13 +3161,13 @@
       <c r="H12" s="10">
         <v>5</v>
       </c>
-      <c r="I12" s="118"/>
+      <c r="I12" s="125"/>
       <c r="J12" s="114"/>
     </row>
     <row r="13" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="130"/>
-      <c r="B13" s="118"/>
-      <c r="C13" s="125"/>
+      <c r="A13" s="117"/>
+      <c r="B13" s="125"/>
+      <c r="C13" s="129"/>
       <c r="D13" s="17" t="s">
         <v>74</v>
       </c>
@@ -3179,13 +3179,13 @@
       <c r="H13" s="10">
         <v>3</v>
       </c>
-      <c r="I13" s="118"/>
+      <c r="I13" s="125"/>
       <c r="J13" s="114"/>
     </row>
     <row r="14" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="130"/>
-      <c r="B14" s="118"/>
-      <c r="C14" s="125"/>
+      <c r="A14" s="117"/>
+      <c r="B14" s="125"/>
+      <c r="C14" s="129"/>
       <c r="D14" s="17" t="s">
         <v>75</v>
       </c>
@@ -3197,13 +3197,13 @@
       <c r="H14" s="10">
         <v>1</v>
       </c>
-      <c r="I14" s="118"/>
+      <c r="I14" s="125"/>
       <c r="J14" s="114"/>
     </row>
     <row r="15" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="130"/>
-      <c r="B15" s="119"/>
-      <c r="C15" s="128"/>
+      <c r="A15" s="117"/>
+      <c r="B15" s="126"/>
+      <c r="C15" s="130"/>
       <c r="D15" s="17" t="s">
         <v>76</v>
       </c>
@@ -3215,18 +3215,18 @@
       <c r="H15" s="10">
         <v>1</v>
       </c>
-      <c r="I15" s="119"/>
-      <c r="J15" s="116"/>
+      <c r="I15" s="126"/>
+      <c r="J15" s="115"/>
     </row>
     <row r="16" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="130" t="s">
+      <c r="A16" s="117" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="117">
+      <c r="B16" s="131">
         <f>funcionalidades!D9</f>
         <v>2.1</v>
       </c>
-      <c r="C16" s="124" t="str">
+      <c r="C16" s="132" t="str">
         <f>funcionalidades!E9</f>
         <v>Cadastro de produtos</v>
       </c>
@@ -3241,13 +3241,13 @@
       <c r="H16" s="10">
         <v>3</v>
       </c>
-      <c r="I16" s="117"/>
+      <c r="I16" s="131"/>
       <c r="J16" s="113"/>
     </row>
     <row r="17" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="130"/>
-      <c r="B17" s="118"/>
-      <c r="C17" s="125"/>
+      <c r="A17" s="117"/>
+      <c r="B17" s="125"/>
+      <c r="C17" s="129"/>
       <c r="D17" s="17" t="s">
         <v>80</v>
       </c>
@@ -3259,13 +3259,13 @@
       <c r="H17" s="10">
         <v>5</v>
       </c>
-      <c r="I17" s="118"/>
+      <c r="I17" s="125"/>
       <c r="J17" s="114"/>
     </row>
     <row r="18" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="130"/>
-      <c r="B18" s="118"/>
-      <c r="C18" s="125"/>
+      <c r="A18" s="117"/>
+      <c r="B18" s="125"/>
+      <c r="C18" s="129"/>
       <c r="D18" s="17" t="s">
         <v>81</v>
       </c>
@@ -3277,13 +3277,13 @@
       <c r="H18" s="10">
         <v>1</v>
       </c>
-      <c r="I18" s="118"/>
+      <c r="I18" s="125"/>
       <c r="J18" s="114"/>
     </row>
     <row r="19" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="130"/>
-      <c r="B19" s="118"/>
-      <c r="C19" s="125"/>
+      <c r="A19" s="117"/>
+      <c r="B19" s="125"/>
+      <c r="C19" s="129"/>
       <c r="D19" s="17" t="s">
         <v>82</v>
       </c>
@@ -3295,13 +3295,13 @@
       <c r="H19" s="10">
         <v>1</v>
       </c>
-      <c r="I19" s="118"/>
+      <c r="I19" s="125"/>
       <c r="J19" s="114"/>
     </row>
     <row r="20" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="130"/>
-      <c r="B20" s="119"/>
-      <c r="C20" s="128"/>
+      <c r="A20" s="117"/>
+      <c r="B20" s="126"/>
+      <c r="C20" s="130"/>
       <c r="D20" s="17" t="s">
         <v>89</v>
       </c>
@@ -3313,16 +3313,16 @@
       <c r="H20" s="10">
         <v>1</v>
       </c>
-      <c r="I20" s="119"/>
-      <c r="J20" s="116"/>
+      <c r="I20" s="126"/>
+      <c r="J20" s="115"/>
     </row>
     <row r="21" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="130"/>
-      <c r="B21" s="117">
+      <c r="A21" s="117"/>
+      <c r="B21" s="131">
         <f>funcionalidades!D10</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="C21" s="124" t="str">
+      <c r="C21" s="132" t="str">
         <f>funcionalidades!E10</f>
         <v>Criar uma página de catalogo de todos os produtos da loja</v>
       </c>
@@ -3337,13 +3337,13 @@
       <c r="H21" s="10">
         <v>5</v>
       </c>
-      <c r="I21" s="117"/>
+      <c r="I21" s="131"/>
       <c r="J21" s="113"/>
     </row>
     <row r="22" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="130"/>
-      <c r="B22" s="118"/>
-      <c r="C22" s="125"/>
+      <c r="A22" s="117"/>
+      <c r="B22" s="125"/>
+      <c r="C22" s="129"/>
       <c r="D22" s="17" t="s">
         <v>84</v>
       </c>
@@ -3355,13 +3355,13 @@
       <c r="H22" s="10">
         <v>1</v>
       </c>
-      <c r="I22" s="118"/>
+      <c r="I22" s="125"/>
       <c r="J22" s="114"/>
     </row>
     <row r="23" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="130"/>
-      <c r="B23" s="118"/>
-      <c r="C23" s="125"/>
+      <c r="A23" s="117"/>
+      <c r="B23" s="125"/>
+      <c r="C23" s="129"/>
       <c r="D23" s="17" t="s">
         <v>85</v>
       </c>
@@ -3373,13 +3373,13 @@
       <c r="H23" s="10">
         <v>1</v>
       </c>
-      <c r="I23" s="118"/>
+      <c r="I23" s="125"/>
       <c r="J23" s="114"/>
     </row>
     <row r="24" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="130"/>
-      <c r="B24" s="119"/>
-      <c r="C24" s="128"/>
+      <c r="A24" s="117"/>
+      <c r="B24" s="126"/>
+      <c r="C24" s="130"/>
       <c r="D24" s="17" t="s">
         <v>86</v>
       </c>
@@ -3391,17 +3391,17 @@
       <c r="H24" s="10">
         <v>1</v>
       </c>
-      <c r="I24" s="119"/>
-      <c r="J24" s="116"/>
+      <c r="I24" s="126"/>
+      <c r="J24" s="115"/>
     </row>
     <row r="25" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="130" t="s">
+      <c r="A25" s="117" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="117">
+      <c r="B25" s="131">
         <v>3.1</v>
       </c>
-      <c r="C25" s="124" t="str">
+      <c r="C25" s="132" t="str">
         <f>funcionalidades!E11</f>
         <v>Criar uma página de vendas</v>
       </c>
@@ -3416,13 +3416,13 @@
       <c r="H25" s="10">
         <v>3</v>
       </c>
-      <c r="I25" s="117"/>
+      <c r="I25" s="131"/>
       <c r="J25" s="113"/>
     </row>
     <row r="26" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="130"/>
-      <c r="B26" s="118"/>
-      <c r="C26" s="125"/>
+      <c r="A26" s="117"/>
+      <c r="B26" s="125"/>
+      <c r="C26" s="129"/>
       <c r="D26" s="17" t="s">
         <v>110</v>
       </c>
@@ -3434,13 +3434,13 @@
       <c r="H26" s="10">
         <v>1</v>
       </c>
-      <c r="I26" s="118"/>
+      <c r="I26" s="125"/>
       <c r="J26" s="114"/>
     </row>
     <row r="27" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="130"/>
-      <c r="B27" s="118"/>
-      <c r="C27" s="125"/>
+      <c r="A27" s="117"/>
+      <c r="B27" s="125"/>
+      <c r="C27" s="129"/>
       <c r="D27" s="17" t="s">
         <v>111</v>
       </c>
@@ -3452,13 +3452,13 @@
       <c r="H27" s="10">
         <v>1</v>
       </c>
-      <c r="I27" s="118"/>
+      <c r="I27" s="125"/>
       <c r="J27" s="114"/>
     </row>
     <row r="28" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="130"/>
-      <c r="B28" s="119"/>
-      <c r="C28" s="128"/>
+      <c r="A28" s="117"/>
+      <c r="B28" s="126"/>
+      <c r="C28" s="130"/>
       <c r="D28" s="17" t="s">
         <v>112</v>
       </c>
@@ -3470,15 +3470,15 @@
       <c r="H28" s="10">
         <v>1</v>
       </c>
-      <c r="I28" s="119"/>
-      <c r="J28" s="116"/>
+      <c r="I28" s="126"/>
+      <c r="J28" s="115"/>
     </row>
     <row r="29" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="130"/>
-      <c r="B29" s="117">
+      <c r="A29" s="117"/>
+      <c r="B29" s="131">
         <v>3.2</v>
       </c>
-      <c r="C29" s="124" t="str">
+      <c r="C29" s="132" t="str">
         <f>funcionalidades!E12</f>
         <v>Criar o cadastro de clientes</v>
       </c>
@@ -3493,13 +3493,13 @@
       <c r="H29" s="10">
         <v>3</v>
       </c>
-      <c r="I29" s="117"/>
+      <c r="I29" s="131"/>
       <c r="J29" s="113"/>
     </row>
     <row r="30" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="130"/>
-      <c r="B30" s="118"/>
-      <c r="C30" s="125"/>
+      <c r="A30" s="117"/>
+      <c r="B30" s="125"/>
+      <c r="C30" s="129"/>
       <c r="D30" s="17" t="s">
         <v>114</v>
       </c>
@@ -3511,13 +3511,13 @@
       <c r="H30" s="10">
         <v>3</v>
       </c>
-      <c r="I30" s="118"/>
+      <c r="I30" s="125"/>
       <c r="J30" s="114"/>
     </row>
     <row r="31" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="130"/>
-      <c r="B31" s="118"/>
-      <c r="C31" s="125"/>
+      <c r="A31" s="117"/>
+      <c r="B31" s="125"/>
+      <c r="C31" s="129"/>
       <c r="D31" s="17" t="s">
         <v>114</v>
       </c>
@@ -3529,13 +3529,13 @@
       <c r="H31" s="10">
         <v>1</v>
       </c>
-      <c r="I31" s="118"/>
+      <c r="I31" s="125"/>
       <c r="J31" s="114"/>
     </row>
     <row r="32" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="130"/>
-      <c r="B32" s="118"/>
-      <c r="C32" s="125"/>
+      <c r="A32" s="117"/>
+      <c r="B32" s="125"/>
+      <c r="C32" s="129"/>
       <c r="D32" s="17" t="s">
         <v>115</v>
       </c>
@@ -3547,13 +3547,13 @@
       <c r="H32" s="10">
         <v>1</v>
       </c>
-      <c r="I32" s="118"/>
+      <c r="I32" s="125"/>
       <c r="J32" s="114"/>
     </row>
     <row r="33" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="130"/>
-      <c r="B33" s="119"/>
-      <c r="C33" s="128"/>
+      <c r="A33" s="117"/>
+      <c r="B33" s="126"/>
+      <c r="C33" s="130"/>
       <c r="D33" s="17" t="s">
         <v>116</v>
       </c>
@@ -3565,16 +3565,16 @@
       <c r="H33" s="10">
         <v>1</v>
       </c>
-      <c r="I33" s="119"/>
-      <c r="J33" s="116"/>
+      <c r="I33" s="126"/>
+      <c r="J33" s="115"/>
     </row>
     <row r="34" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="130"/>
-      <c r="B34" s="117">
+      <c r="A34" s="117"/>
+      <c r="B34" s="131">
         <f>funcionalidades!D13</f>
         <v>3.3</v>
       </c>
-      <c r="C34" s="124" t="str">
+      <c r="C34" s="132" t="str">
         <f>funcionalidades!E13</f>
         <v>Criar carrinho de compras</v>
       </c>
@@ -3589,13 +3589,13 @@
       <c r="H34" s="10">
         <v>3</v>
       </c>
-      <c r="I34" s="117"/>
+      <c r="I34" s="131"/>
       <c r="J34" s="113"/>
     </row>
     <row r="35" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="130"/>
-      <c r="B35" s="118"/>
-      <c r="C35" s="125"/>
+      <c r="A35" s="117"/>
+      <c r="B35" s="125"/>
+      <c r="C35" s="129"/>
       <c r="D35" s="17" t="s">
         <v>118</v>
       </c>
@@ -3607,13 +3607,13 @@
       <c r="H35" s="10">
         <v>5</v>
       </c>
-      <c r="I35" s="118"/>
+      <c r="I35" s="125"/>
       <c r="J35" s="114"/>
     </row>
     <row r="36" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="130"/>
-      <c r="B36" s="118"/>
-      <c r="C36" s="125"/>
+      <c r="A36" s="117"/>
+      <c r="B36" s="125"/>
+      <c r="C36" s="129"/>
       <c r="D36" s="17" t="s">
         <v>119</v>
       </c>
@@ -3625,13 +3625,13 @@
       <c r="H36" s="10">
         <v>1</v>
       </c>
-      <c r="I36" s="118"/>
+      <c r="I36" s="125"/>
       <c r="J36" s="114"/>
     </row>
     <row r="37" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="130"/>
-      <c r="B37" s="118"/>
-      <c r="C37" s="125"/>
+      <c r="A37" s="117"/>
+      <c r="B37" s="125"/>
+      <c r="C37" s="129"/>
       <c r="D37" s="17" t="s">
         <v>120</v>
       </c>
@@ -3643,13 +3643,13 @@
       <c r="H37" s="10">
         <v>1</v>
       </c>
-      <c r="I37" s="118"/>
+      <c r="I37" s="125"/>
       <c r="J37" s="114"/>
     </row>
     <row r="38" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="130"/>
-      <c r="B38" s="119"/>
-      <c r="C38" s="128"/>
+      <c r="A38" s="117"/>
+      <c r="B38" s="126"/>
+      <c r="C38" s="130"/>
       <c r="D38" s="17" t="s">
         <v>121</v>
       </c>
@@ -3661,18 +3661,18 @@
       <c r="H38" s="10">
         <v>1</v>
       </c>
-      <c r="I38" s="119"/>
-      <c r="J38" s="116"/>
+      <c r="I38" s="126"/>
+      <c r="J38" s="115"/>
     </row>
     <row r="39" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="120" t="s">
+      <c r="A39" s="133" t="s">
         <v>9</v>
       </c>
-      <c r="B39" s="117">
+      <c r="B39" s="131">
         <f>funcionalidades!D14</f>
         <v>4.0999999999999996</v>
       </c>
-      <c r="C39" s="124" t="str">
+      <c r="C39" s="132" t="str">
         <f>funcionalidades!E14</f>
         <v>Gestão dos consultores</v>
       </c>
@@ -3687,13 +3687,13 @@
       <c r="H39" s="10">
         <v>3</v>
       </c>
-      <c r="I39" s="117"/>
+      <c r="I39" s="131"/>
       <c r="J39" s="113"/>
     </row>
     <row r="40" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="121"/>
-      <c r="B40" s="118"/>
-      <c r="C40" s="125"/>
+      <c r="A40" s="134"/>
+      <c r="B40" s="125"/>
+      <c r="C40" s="129"/>
       <c r="D40" s="17" t="s">
         <v>138</v>
       </c>
@@ -3705,13 +3705,13 @@
       <c r="H40" s="10">
         <v>3</v>
       </c>
-      <c r="I40" s="118"/>
+      <c r="I40" s="125"/>
       <c r="J40" s="114"/>
     </row>
     <row r="41" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="121"/>
-      <c r="B41" s="118"/>
-      <c r="C41" s="125"/>
+      <c r="A41" s="134"/>
+      <c r="B41" s="125"/>
+      <c r="C41" s="129"/>
       <c r="D41" s="17" t="s">
         <v>139</v>
       </c>
@@ -3721,13 +3721,13 @@
       <c r="F41" s="10"/>
       <c r="G41" s="11"/>
       <c r="H41" s="11"/>
-      <c r="I41" s="118"/>
+      <c r="I41" s="125"/>
       <c r="J41" s="114"/>
     </row>
     <row r="42" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="121"/>
-      <c r="B42" s="118"/>
-      <c r="C42" s="125"/>
+      <c r="A42" s="134"/>
+      <c r="B42" s="125"/>
+      <c r="C42" s="129"/>
       <c r="D42" s="17" t="s">
         <v>126</v>
       </c>
@@ -3737,13 +3737,13 @@
       <c r="F42" s="10"/>
       <c r="G42" s="11"/>
       <c r="H42" s="11"/>
-      <c r="I42" s="118"/>
+      <c r="I42" s="125"/>
       <c r="J42" s="114"/>
     </row>
     <row r="43" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="121"/>
-      <c r="B43" s="118"/>
-      <c r="C43" s="125"/>
+      <c r="A43" s="134"/>
+      <c r="B43" s="125"/>
+      <c r="C43" s="129"/>
       <c r="D43" s="17" t="s">
         <v>140</v>
       </c>
@@ -3753,13 +3753,13 @@
       <c r="F43" s="10"/>
       <c r="G43" s="11"/>
       <c r="H43" s="11"/>
-      <c r="I43" s="118"/>
+      <c r="I43" s="125"/>
       <c r="J43" s="114"/>
     </row>
     <row r="44" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="121"/>
-      <c r="B44" s="118"/>
-      <c r="C44" s="125"/>
+      <c r="A44" s="134"/>
+      <c r="B44" s="125"/>
+      <c r="C44" s="129"/>
       <c r="D44" s="17" t="s">
         <v>141</v>
       </c>
@@ -3769,13 +3769,13 @@
       <c r="F44" s="10"/>
       <c r="G44" s="11"/>
       <c r="H44" s="11"/>
-      <c r="I44" s="118"/>
+      <c r="I44" s="125"/>
       <c r="J44" s="114"/>
     </row>
     <row r="45" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="127"/>
-      <c r="B45" s="119"/>
-      <c r="C45" s="128"/>
+      <c r="A45" s="135"/>
+      <c r="B45" s="126"/>
+      <c r="C45" s="130"/>
       <c r="D45" s="17" t="s">
         <v>142</v>
       </c>
@@ -3785,18 +3785,18 @@
       <c r="F45" s="10"/>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
-      <c r="I45" s="119"/>
-      <c r="J45" s="116"/>
+      <c r="I45" s="126"/>
+      <c r="J45" s="115"/>
     </row>
     <row r="46" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="120" t="s">
+      <c r="A46" s="133" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="117">
+      <c r="B46" s="131">
         <f>funcionalidades!D15</f>
         <v>5.0999999999999996</v>
       </c>
-      <c r="C46" s="124" t="str">
+      <c r="C46" s="132" t="str">
         <f>funcionalidades!E15</f>
         <v>Área de acesso dos consultores</v>
       </c>
@@ -3809,13 +3809,13 @@
       <c r="F46" s="10"/>
       <c r="G46" s="11"/>
       <c r="H46" s="11"/>
-      <c r="I46" s="117"/>
+      <c r="I46" s="131"/>
       <c r="J46" s="113"/>
     </row>
     <row r="47" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="121"/>
-      <c r="B47" s="118"/>
-      <c r="C47" s="125"/>
+      <c r="A47" s="134"/>
+      <c r="B47" s="125"/>
+      <c r="C47" s="129"/>
       <c r="D47" s="17" t="s">
         <v>144</v>
       </c>
@@ -3825,13 +3825,13 @@
       <c r="F47" s="10"/>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
-      <c r="I47" s="118"/>
+      <c r="I47" s="125"/>
       <c r="J47" s="114"/>
     </row>
     <row r="48" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="121"/>
-      <c r="B48" s="118"/>
-      <c r="C48" s="125"/>
+      <c r="A48" s="134"/>
+      <c r="B48" s="125"/>
+      <c r="C48" s="129"/>
       <c r="D48" s="17" t="s">
         <v>145</v>
       </c>
@@ -3841,13 +3841,13 @@
       <c r="F48" s="10"/>
       <c r="G48" s="11"/>
       <c r="H48" s="11"/>
-      <c r="I48" s="118"/>
+      <c r="I48" s="125"/>
       <c r="J48" s="114"/>
     </row>
     <row r="49" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="121"/>
-      <c r="B49" s="118"/>
-      <c r="C49" s="125"/>
+      <c r="A49" s="134"/>
+      <c r="B49" s="125"/>
+      <c r="C49" s="129"/>
       <c r="D49" s="17" t="s">
         <v>146</v>
       </c>
@@ -3857,13 +3857,13 @@
       <c r="F49" s="10"/>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
-      <c r="I49" s="118"/>
+      <c r="I49" s="125"/>
       <c r="J49" s="114"/>
     </row>
     <row r="50" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A50" s="127"/>
-      <c r="B50" s="119"/>
-      <c r="C50" s="128"/>
+      <c r="A50" s="135"/>
+      <c r="B50" s="126"/>
+      <c r="C50" s="130"/>
       <c r="D50" s="17" t="s">
         <v>147</v>
       </c>
@@ -3873,18 +3873,18 @@
       <c r="F50" s="10"/>
       <c r="G50" s="11"/>
       <c r="H50" s="11"/>
-      <c r="I50" s="119"/>
-      <c r="J50" s="116"/>
+      <c r="I50" s="126"/>
+      <c r="J50" s="115"/>
     </row>
     <row r="51" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="120" t="s">
+      <c r="A51" s="133" t="s">
         <v>196</v>
       </c>
-      <c r="B51" s="117">
+      <c r="B51" s="131">
         <f>funcionalidades!D16</f>
         <v>6.1</v>
       </c>
-      <c r="C51" s="124" t="str">
+      <c r="C51" s="132" t="str">
         <f>funcionalidades!E16</f>
         <v>Cadastro de Funcionarios</v>
       </c>
@@ -3897,13 +3897,13 @@
       <c r="F51" s="10"/>
       <c r="G51" s="11"/>
       <c r="H51" s="11"/>
-      <c r="I51" s="117"/>
+      <c r="I51" s="131"/>
       <c r="J51" s="113"/>
     </row>
     <row r="52" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="121"/>
-      <c r="B52" s="118"/>
-      <c r="C52" s="125"/>
+      <c r="A52" s="134"/>
+      <c r="B52" s="125"/>
+      <c r="C52" s="129"/>
       <c r="D52" s="17" t="s">
         <v>149</v>
       </c>
@@ -3913,13 +3913,13 @@
       <c r="F52" s="10"/>
       <c r="G52" s="11"/>
       <c r="H52" s="11"/>
-      <c r="I52" s="118"/>
+      <c r="I52" s="125"/>
       <c r="J52" s="114"/>
     </row>
     <row r="53" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="121"/>
-      <c r="B53" s="118"/>
-      <c r="C53" s="125"/>
+      <c r="A53" s="134"/>
+      <c r="B53" s="125"/>
+      <c r="C53" s="129"/>
       <c r="D53" s="17" t="s">
         <v>152</v>
       </c>
@@ -3929,13 +3929,13 @@
       <c r="F53" s="10"/>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
-      <c r="I53" s="118"/>
+      <c r="I53" s="125"/>
       <c r="J53" s="114"/>
     </row>
     <row r="54" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A54" s="121"/>
-      <c r="B54" s="118"/>
-      <c r="C54" s="125"/>
+      <c r="A54" s="134"/>
+      <c r="B54" s="125"/>
+      <c r="C54" s="129"/>
       <c r="D54" s="17" t="s">
         <v>153</v>
       </c>
@@ -3945,13 +3945,13 @@
       <c r="F54" s="10"/>
       <c r="G54" s="11"/>
       <c r="H54" s="11"/>
-      <c r="I54" s="118"/>
+      <c r="I54" s="125"/>
       <c r="J54" s="114"/>
     </row>
     <row r="55" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A55" s="121"/>
-      <c r="B55" s="119"/>
-      <c r="C55" s="128"/>
+      <c r="A55" s="134"/>
+      <c r="B55" s="126"/>
+      <c r="C55" s="130"/>
       <c r="D55" s="17" t="s">
         <v>154</v>
       </c>
@@ -3961,16 +3961,16 @@
       <c r="F55" s="10"/>
       <c r="G55" s="11"/>
       <c r="H55" s="11"/>
-      <c r="I55" s="119"/>
-      <c r="J55" s="116"/>
+      <c r="I55" s="126"/>
+      <c r="J55" s="115"/>
     </row>
     <row r="56" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="121"/>
-      <c r="B56" s="117">
+      <c r="A56" s="134"/>
+      <c r="B56" s="131">
         <f>funcionalidades!D17</f>
         <v>6.2</v>
       </c>
-      <c r="C56" s="124" t="str">
+      <c r="C56" s="132" t="str">
         <f>funcionalidades!E17</f>
         <v>Controle de estoque</v>
       </c>
@@ -3983,13 +3983,13 @@
       <c r="F56" s="10"/>
       <c r="G56" s="11"/>
       <c r="H56" s="11"/>
-      <c r="I56" s="117"/>
+      <c r="I56" s="131"/>
       <c r="J56" s="113"/>
     </row>
     <row r="57" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="121"/>
-      <c r="B57" s="118"/>
-      <c r="C57" s="125"/>
+      <c r="A57" s="134"/>
+      <c r="B57" s="125"/>
+      <c r="C57" s="129"/>
       <c r="D57" s="17" t="s">
         <v>164</v>
       </c>
@@ -3999,13 +3999,13 @@
       <c r="F57" s="10"/>
       <c r="G57" s="11"/>
       <c r="H57" s="11"/>
-      <c r="I57" s="118"/>
+      <c r="I57" s="125"/>
       <c r="J57" s="114"/>
     </row>
     <row r="58" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A58" s="121"/>
-      <c r="B58" s="118"/>
-      <c r="C58" s="125"/>
+      <c r="A58" s="134"/>
+      <c r="B58" s="125"/>
+      <c r="C58" s="129"/>
       <c r="D58" s="17" t="s">
         <v>165</v>
       </c>
@@ -4015,13 +4015,13 @@
       <c r="F58" s="10"/>
       <c r="G58" s="11"/>
       <c r="H58" s="11"/>
-      <c r="I58" s="118"/>
+      <c r="I58" s="125"/>
       <c r="J58" s="114"/>
     </row>
     <row r="59" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="121"/>
-      <c r="B59" s="119"/>
-      <c r="C59" s="128"/>
+      <c r="A59" s="134"/>
+      <c r="B59" s="126"/>
+      <c r="C59" s="130"/>
       <c r="D59" s="17" t="s">
         <v>166</v>
       </c>
@@ -4031,16 +4031,16 @@
       <c r="F59" s="10"/>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
-      <c r="I59" s="119"/>
-      <c r="J59" s="116"/>
+      <c r="I59" s="126"/>
+      <c r="J59" s="115"/>
     </row>
     <row r="60" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A60" s="121"/>
-      <c r="B60" s="117">
+      <c r="A60" s="134"/>
+      <c r="B60" s="131">
         <f>funcionalidades!D18</f>
         <v>6.3</v>
       </c>
-      <c r="C60" s="124" t="str">
+      <c r="C60" s="132" t="str">
         <f>funcionalidades!E18</f>
         <v>Categorias de usuário</v>
       </c>
@@ -4053,13 +4053,13 @@
       <c r="F60" s="10"/>
       <c r="G60" s="11"/>
       <c r="H60" s="11"/>
-      <c r="I60" s="117"/>
+      <c r="I60" s="131"/>
       <c r="J60" s="113"/>
     </row>
     <row r="61" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A61" s="121"/>
-      <c r="B61" s="118"/>
-      <c r="C61" s="125"/>
+      <c r="A61" s="134"/>
+      <c r="B61" s="125"/>
+      <c r="C61" s="129"/>
       <c r="D61" s="17" t="s">
         <v>168</v>
       </c>
@@ -4069,13 +4069,13 @@
       <c r="F61" s="10"/>
       <c r="G61" s="11"/>
       <c r="H61" s="11"/>
-      <c r="I61" s="118"/>
+      <c r="I61" s="125"/>
       <c r="J61" s="114"/>
     </row>
     <row r="62" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A62" s="121"/>
-      <c r="B62" s="118"/>
-      <c r="C62" s="125"/>
+      <c r="A62" s="134"/>
+      <c r="B62" s="125"/>
+      <c r="C62" s="129"/>
       <c r="D62" s="17" t="s">
         <v>169</v>
       </c>
@@ -4085,13 +4085,13 @@
       <c r="F62" s="10"/>
       <c r="G62" s="11"/>
       <c r="H62" s="11"/>
-      <c r="I62" s="118"/>
+      <c r="I62" s="125"/>
       <c r="J62" s="114"/>
     </row>
     <row r="63" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A63" s="121"/>
-      <c r="B63" s="118"/>
-      <c r="C63" s="125"/>
+      <c r="A63" s="134"/>
+      <c r="B63" s="125"/>
+      <c r="C63" s="129"/>
       <c r="D63" s="17" t="s">
         <v>170</v>
       </c>
@@ -4101,13 +4101,13 @@
       <c r="F63" s="10"/>
       <c r="G63" s="11"/>
       <c r="H63" s="11"/>
-      <c r="I63" s="118"/>
+      <c r="I63" s="125"/>
       <c r="J63" s="114"/>
     </row>
     <row r="64" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A64" s="121"/>
-      <c r="B64" s="119"/>
-      <c r="C64" s="128"/>
+      <c r="A64" s="134"/>
+      <c r="B64" s="126"/>
+      <c r="C64" s="130"/>
       <c r="D64" s="17" t="s">
         <v>171</v>
       </c>
@@ -4117,16 +4117,16 @@
       <c r="F64" s="10"/>
       <c r="G64" s="11"/>
       <c r="H64" s="11"/>
-      <c r="I64" s="119"/>
-      <c r="J64" s="116"/>
+      <c r="I64" s="126"/>
+      <c r="J64" s="115"/>
     </row>
     <row r="65" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A65" s="121"/>
-      <c r="B65" s="117">
+      <c r="A65" s="134"/>
+      <c r="B65" s="131">
         <f>funcionalidades!D19</f>
         <v>6.4</v>
       </c>
-      <c r="C65" s="124" t="str">
+      <c r="C65" s="132" t="str">
         <f>funcionalidades!E19</f>
         <v>Terminal de atendimento (PDV)</v>
       </c>
@@ -4139,13 +4139,13 @@
       <c r="F65" s="10"/>
       <c r="G65" s="11"/>
       <c r="H65" s="11"/>
-      <c r="I65" s="117"/>
+      <c r="I65" s="131"/>
       <c r="J65" s="113"/>
     </row>
     <row r="66" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A66" s="121"/>
-      <c r="B66" s="118"/>
-      <c r="C66" s="125"/>
+      <c r="A66" s="134"/>
+      <c r="B66" s="125"/>
+      <c r="C66" s="129"/>
       <c r="D66" s="17" t="s">
         <v>173</v>
       </c>
@@ -4155,13 +4155,13 @@
       <c r="F66" s="10"/>
       <c r="G66" s="11"/>
       <c r="H66" s="11"/>
-      <c r="I66" s="118"/>
+      <c r="I66" s="125"/>
       <c r="J66" s="114"/>
     </row>
     <row r="67" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A67" s="121"/>
-      <c r="B67" s="118"/>
-      <c r="C67" s="125"/>
+      <c r="A67" s="134"/>
+      <c r="B67" s="125"/>
+      <c r="C67" s="129"/>
       <c r="D67" s="17" t="s">
         <v>174</v>
       </c>
@@ -4171,13 +4171,13 @@
       <c r="F67" s="10"/>
       <c r="G67" s="11"/>
       <c r="H67" s="11"/>
-      <c r="I67" s="118"/>
+      <c r="I67" s="125"/>
       <c r="J67" s="114"/>
     </row>
     <row r="68" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A68" s="121"/>
-      <c r="B68" s="118"/>
-      <c r="C68" s="125"/>
+      <c r="A68" s="134"/>
+      <c r="B68" s="125"/>
+      <c r="C68" s="129"/>
       <c r="D68" s="17" t="s">
         <v>175</v>
       </c>
@@ -4187,13 +4187,13 @@
       <c r="F68" s="10"/>
       <c r="G68" s="11"/>
       <c r="H68" s="11"/>
-      <c r="I68" s="118"/>
+      <c r="I68" s="125"/>
       <c r="J68" s="114"/>
     </row>
     <row r="69" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A69" s="121"/>
-      <c r="B69" s="119"/>
-      <c r="C69" s="128"/>
+      <c r="A69" s="134"/>
+      <c r="B69" s="126"/>
+      <c r="C69" s="130"/>
       <c r="D69" s="17" t="s">
         <v>176</v>
       </c>
@@ -4203,16 +4203,16 @@
       <c r="F69" s="10"/>
       <c r="G69" s="11"/>
       <c r="H69" s="11"/>
-      <c r="I69" s="119"/>
-      <c r="J69" s="116"/>
+      <c r="I69" s="126"/>
+      <c r="J69" s="115"/>
     </row>
     <row r="70" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A70" s="121"/>
-      <c r="B70" s="117">
+      <c r="A70" s="134"/>
+      <c r="B70" s="131">
         <f>funcionalidades!D20</f>
         <v>6.5</v>
       </c>
-      <c r="C70" s="124" t="str">
+      <c r="C70" s="132" t="str">
         <f>funcionalidades!E20</f>
         <v>Controle das vendas</v>
       </c>
@@ -4225,13 +4225,13 @@
       <c r="F70" s="10"/>
       <c r="G70" s="11"/>
       <c r="H70" s="11"/>
-      <c r="I70" s="117"/>
+      <c r="I70" s="131"/>
       <c r="J70" s="113"/>
     </row>
     <row r="71" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A71" s="121"/>
-      <c r="B71" s="118"/>
-      <c r="C71" s="125"/>
+      <c r="A71" s="134"/>
+      <c r="B71" s="125"/>
+      <c r="C71" s="129"/>
       <c r="D71" s="17" t="s">
         <v>178</v>
       </c>
@@ -4241,13 +4241,13 @@
       <c r="F71" s="10"/>
       <c r="G71" s="11"/>
       <c r="H71" s="11"/>
-      <c r="I71" s="118"/>
+      <c r="I71" s="125"/>
       <c r="J71" s="114"/>
     </row>
     <row r="72" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A72" s="121"/>
-      <c r="B72" s="118"/>
-      <c r="C72" s="125"/>
+      <c r="A72" s="134"/>
+      <c r="B72" s="125"/>
+      <c r="C72" s="129"/>
       <c r="D72" s="17" t="s">
         <v>179</v>
       </c>
@@ -4257,13 +4257,13 @@
       <c r="F72" s="10"/>
       <c r="G72" s="11"/>
       <c r="H72" s="11"/>
-      <c r="I72" s="118"/>
+      <c r="I72" s="125"/>
       <c r="J72" s="114"/>
     </row>
     <row r="73" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="121"/>
-      <c r="B73" s="119"/>
-      <c r="C73" s="128"/>
+      <c r="A73" s="134"/>
+      <c r="B73" s="126"/>
+      <c r="C73" s="130"/>
       <c r="D73" s="17" t="s">
         <v>180</v>
       </c>
@@ -4273,16 +4273,16 @@
       <c r="F73" s="10"/>
       <c r="G73" s="11"/>
       <c r="H73" s="11"/>
-      <c r="I73" s="119"/>
-      <c r="J73" s="116"/>
+      <c r="I73" s="126"/>
+      <c r="J73" s="115"/>
     </row>
     <row r="74" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="121"/>
-      <c r="B74" s="117">
+      <c r="A74" s="134"/>
+      <c r="B74" s="131">
         <f>funcionalidades!D21</f>
         <v>6.6</v>
       </c>
-      <c r="C74" s="124" t="str">
+      <c r="C74" s="132" t="str">
         <f>funcionalidades!E21</f>
         <v>Gestão das comissões</v>
       </c>
@@ -4295,13 +4295,13 @@
       <c r="F74" s="10"/>
       <c r="G74" s="11"/>
       <c r="H74" s="11"/>
-      <c r="I74" s="117"/>
+      <c r="I74" s="131"/>
       <c r="J74" s="113"/>
     </row>
     <row r="75" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A75" s="121"/>
-      <c r="B75" s="118"/>
-      <c r="C75" s="125"/>
+      <c r="A75" s="134"/>
+      <c r="B75" s="125"/>
+      <c r="C75" s="129"/>
       <c r="D75" s="17" t="s">
         <v>182</v>
       </c>
@@ -4311,13 +4311,13 @@
       <c r="F75" s="10"/>
       <c r="G75" s="11"/>
       <c r="H75" s="11"/>
-      <c r="I75" s="118"/>
+      <c r="I75" s="125"/>
       <c r="J75" s="114"/>
     </row>
     <row r="76" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A76" s="121"/>
-      <c r="B76" s="118"/>
-      <c r="C76" s="125"/>
+      <c r="A76" s="134"/>
+      <c r="B76" s="125"/>
+      <c r="C76" s="129"/>
       <c r="D76" s="17" t="s">
         <v>183</v>
       </c>
@@ -4327,13 +4327,13 @@
       <c r="F76" s="10"/>
       <c r="G76" s="11"/>
       <c r="H76" s="11"/>
-      <c r="I76" s="118"/>
+      <c r="I76" s="125"/>
       <c r="J76" s="114"/>
     </row>
     <row r="77" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A77" s="127"/>
-      <c r="B77" s="119"/>
-      <c r="C77" s="128"/>
+      <c r="A77" s="135"/>
+      <c r="B77" s="126"/>
+      <c r="C77" s="130"/>
       <c r="D77" s="17" t="s">
         <v>184</v>
       </c>
@@ -4343,18 +4343,18 @@
       <c r="F77" s="10"/>
       <c r="G77" s="11"/>
       <c r="H77" s="11"/>
-      <c r="I77" s="119"/>
-      <c r="J77" s="116"/>
+      <c r="I77" s="126"/>
+      <c r="J77" s="115"/>
     </row>
     <row r="78" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A78" s="120" t="s">
+      <c r="A78" s="133" t="s">
         <v>136</v>
       </c>
-      <c r="B78" s="117">
+      <c r="B78" s="131">
         <f>funcionalidades!D22</f>
         <v>7.1</v>
       </c>
-      <c r="C78" s="124" t="str">
+      <c r="C78" s="132" t="str">
         <f>funcionalidades!E22</f>
         <v>Cadastro de Fornecedores</v>
       </c>
@@ -4367,13 +4367,13 @@
       <c r="F78" s="10"/>
       <c r="G78" s="11"/>
       <c r="H78" s="11"/>
-      <c r="I78" s="117"/>
+      <c r="I78" s="131"/>
       <c r="J78" s="113"/>
     </row>
     <row r="79" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A79" s="121"/>
-      <c r="B79" s="118"/>
-      <c r="C79" s="125"/>
+      <c r="A79" s="134"/>
+      <c r="B79" s="125"/>
+      <c r="C79" s="129"/>
       <c r="D79" s="17" t="s">
         <v>190</v>
       </c>
@@ -4383,13 +4383,13 @@
       <c r="F79" s="10"/>
       <c r="G79" s="11"/>
       <c r="H79" s="11"/>
-      <c r="I79" s="118"/>
+      <c r="I79" s="125"/>
       <c r="J79" s="114"/>
     </row>
     <row r="80" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A80" s="121"/>
-      <c r="B80" s="118"/>
-      <c r="C80" s="125"/>
+      <c r="A80" s="134"/>
+      <c r="B80" s="125"/>
+      <c r="C80" s="129"/>
       <c r="D80" s="17" t="s">
         <v>191</v>
       </c>
@@ -4399,13 +4399,13 @@
       <c r="F80" s="10"/>
       <c r="G80" s="11"/>
       <c r="H80" s="11"/>
-      <c r="I80" s="118"/>
+      <c r="I80" s="125"/>
       <c r="J80" s="114"/>
     </row>
     <row r="81" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A81" s="121"/>
-      <c r="B81" s="118"/>
-      <c r="C81" s="125"/>
+      <c r="A81" s="134"/>
+      <c r="B81" s="125"/>
+      <c r="C81" s="129"/>
       <c r="D81" s="17" t="s">
         <v>192</v>
       </c>
@@ -4415,13 +4415,13 @@
       <c r="F81" s="10"/>
       <c r="G81" s="11"/>
       <c r="H81" s="11"/>
-      <c r="I81" s="118"/>
+      <c r="I81" s="125"/>
       <c r="J81" s="114"/>
     </row>
     <row r="82" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A82" s="121"/>
-      <c r="B82" s="118"/>
-      <c r="C82" s="125"/>
+      <c r="A82" s="134"/>
+      <c r="B82" s="125"/>
+      <c r="C82" s="129"/>
       <c r="D82" s="17" t="s">
         <v>193</v>
       </c>
@@ -4431,13 +4431,13 @@
       <c r="F82" s="10"/>
       <c r="G82" s="11"/>
       <c r="H82" s="11"/>
-      <c r="I82" s="118"/>
+      <c r="I82" s="125"/>
       <c r="J82" s="114"/>
     </row>
     <row r="83" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A83" s="121"/>
-      <c r="B83" s="118"/>
-      <c r="C83" s="125"/>
+      <c r="A83" s="134"/>
+      <c r="B83" s="125"/>
+      <c r="C83" s="129"/>
       <c r="D83" s="17" t="s">
         <v>194</v>
       </c>
@@ -4447,13 +4447,13 @@
       <c r="F83" s="10"/>
       <c r="G83" s="11"/>
       <c r="H83" s="11"/>
-      <c r="I83" s="118"/>
+      <c r="I83" s="125"/>
       <c r="J83" s="114"/>
     </row>
     <row r="84" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="122"/>
-      <c r="B84" s="123"/>
-      <c r="C84" s="126"/>
+      <c r="A84" s="136"/>
+      <c r="B84" s="137"/>
+      <c r="C84" s="138"/>
       <c r="D84" s="35" t="s">
         <v>195</v>
       </c>
@@ -4463,8 +4463,8 @@
       <c r="F84" s="36"/>
       <c r="G84" s="37"/>
       <c r="H84" s="37"/>
-      <c r="I84" s="123"/>
-      <c r="J84" s="115"/>
+      <c r="I84" s="137"/>
+      <c r="J84" s="139"/>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="I85" s="1"/>
@@ -4486,6 +4486,60 @@
     </row>
   </sheetData>
   <mergeCells count="70">
+    <mergeCell ref="J78:J84"/>
+    <mergeCell ref="J65:J69"/>
+    <mergeCell ref="I70:I73"/>
+    <mergeCell ref="J70:J73"/>
+    <mergeCell ref="I74:I77"/>
+    <mergeCell ref="J74:J77"/>
+    <mergeCell ref="J51:J55"/>
+    <mergeCell ref="I56:I59"/>
+    <mergeCell ref="J56:J59"/>
+    <mergeCell ref="I60:I64"/>
+    <mergeCell ref="J60:J64"/>
+    <mergeCell ref="J34:J38"/>
+    <mergeCell ref="I39:I45"/>
+    <mergeCell ref="J39:J45"/>
+    <mergeCell ref="I46:I50"/>
+    <mergeCell ref="J46:J50"/>
+    <mergeCell ref="J21:J24"/>
+    <mergeCell ref="I25:I28"/>
+    <mergeCell ref="J25:J28"/>
+    <mergeCell ref="I29:I33"/>
+    <mergeCell ref="J29:J33"/>
+    <mergeCell ref="A78:A84"/>
+    <mergeCell ref="B78:B84"/>
+    <mergeCell ref="C78:C84"/>
+    <mergeCell ref="A51:A77"/>
+    <mergeCell ref="I16:I20"/>
+    <mergeCell ref="I21:I24"/>
+    <mergeCell ref="I34:I38"/>
+    <mergeCell ref="I51:I55"/>
+    <mergeCell ref="I65:I69"/>
+    <mergeCell ref="I78:I84"/>
+    <mergeCell ref="B74:B77"/>
+    <mergeCell ref="C74:C77"/>
+    <mergeCell ref="C60:C64"/>
+    <mergeCell ref="B65:B69"/>
+    <mergeCell ref="C65:C69"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="C46:C50"/>
+    <mergeCell ref="B46:B50"/>
+    <mergeCell ref="A39:A45"/>
+    <mergeCell ref="A46:A50"/>
+    <mergeCell ref="B51:B55"/>
+    <mergeCell ref="C51:C55"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="C56:C59"/>
+    <mergeCell ref="B60:B64"/>
+    <mergeCell ref="C39:C45"/>
+    <mergeCell ref="B39:B45"/>
+    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="B34:B38"/>
+    <mergeCell ref="C25:C28"/>
+    <mergeCell ref="C29:C33"/>
+    <mergeCell ref="C34:C38"/>
     <mergeCell ref="J16:J20"/>
     <mergeCell ref="A9:A15"/>
     <mergeCell ref="A16:A24"/>
@@ -4502,60 +4556,6 @@
     <mergeCell ref="C16:C20"/>
     <mergeCell ref="C21:C24"/>
     <mergeCell ref="B25:B28"/>
-    <mergeCell ref="B29:B33"/>
-    <mergeCell ref="B34:B38"/>
-    <mergeCell ref="C25:C28"/>
-    <mergeCell ref="C29:C33"/>
-    <mergeCell ref="C34:C38"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="C46:C50"/>
-    <mergeCell ref="B46:B50"/>
-    <mergeCell ref="A39:A45"/>
-    <mergeCell ref="A46:A50"/>
-    <mergeCell ref="B51:B55"/>
-    <mergeCell ref="C51:C55"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="C56:C59"/>
-    <mergeCell ref="B60:B64"/>
-    <mergeCell ref="C39:C45"/>
-    <mergeCell ref="B39:B45"/>
-    <mergeCell ref="A78:A84"/>
-    <mergeCell ref="B78:B84"/>
-    <mergeCell ref="C78:C84"/>
-    <mergeCell ref="A51:A77"/>
-    <mergeCell ref="I16:I20"/>
-    <mergeCell ref="I21:I24"/>
-    <mergeCell ref="I34:I38"/>
-    <mergeCell ref="I51:I55"/>
-    <mergeCell ref="I65:I69"/>
-    <mergeCell ref="I78:I84"/>
-    <mergeCell ref="B74:B77"/>
-    <mergeCell ref="C74:C77"/>
-    <mergeCell ref="C60:C64"/>
-    <mergeCell ref="B65:B69"/>
-    <mergeCell ref="C65:C69"/>
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="J21:J24"/>
-    <mergeCell ref="I25:I28"/>
-    <mergeCell ref="J25:J28"/>
-    <mergeCell ref="I29:I33"/>
-    <mergeCell ref="J29:J33"/>
-    <mergeCell ref="J34:J38"/>
-    <mergeCell ref="I39:I45"/>
-    <mergeCell ref="J39:J45"/>
-    <mergeCell ref="I46:I50"/>
-    <mergeCell ref="J46:J50"/>
-    <mergeCell ref="J51:J55"/>
-    <mergeCell ref="I56:I59"/>
-    <mergeCell ref="J56:J59"/>
-    <mergeCell ref="I60:I64"/>
-    <mergeCell ref="J60:J64"/>
-    <mergeCell ref="J78:J84"/>
-    <mergeCell ref="J65:J69"/>
-    <mergeCell ref="I70:I73"/>
-    <mergeCell ref="J70:J73"/>
-    <mergeCell ref="I74:I77"/>
-    <mergeCell ref="J74:J77"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="60" fitToHeight="0" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -6574,8 +6574,8 @@
   </sheetPr>
   <dimension ref="A1:CS30"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:M1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8280,7 +8280,7 @@
         <v>1</v>
       </c>
       <c r="K12" s="33">
-        <f t="shared" ref="K12:K18" si="0">$K$8</f>
+        <f>$K$8</f>
         <v>1</v>
       </c>
       <c r="L12" s="33" t="s">
@@ -8576,7 +8576,7 @@
         <v>2</v>
       </c>
       <c r="K13" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="K12:K18" si="0">$K$8</f>
         <v>1</v>
       </c>
       <c r="L13" s="10" t="s">
@@ -12522,6 +12522,26 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="CG1:CL1"/>
+    <mergeCell ref="CN1:CS1"/>
+    <mergeCell ref="BS10:BX10"/>
+    <mergeCell ref="BZ10:CE10"/>
+    <mergeCell ref="CG10:CL10"/>
+    <mergeCell ref="CN10:CS10"/>
+    <mergeCell ref="BZ1:CE1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="O1:T1"/>
+    <mergeCell ref="O10:T10"/>
+    <mergeCell ref="V1:AA1"/>
+    <mergeCell ref="V10:AA10"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="BE1:BJ1"/>
+    <mergeCell ref="BL1:BQ1"/>
+    <mergeCell ref="BE10:BJ10"/>
+    <mergeCell ref="BL10:BQ10"/>
+    <mergeCell ref="BS1:BX1"/>
     <mergeCell ref="AQ1:AV1"/>
     <mergeCell ref="AX1:BC1"/>
     <mergeCell ref="AQ10:AV10"/>
@@ -12530,26 +12550,6 @@
     <mergeCell ref="AC10:AH10"/>
     <mergeCell ref="AJ1:AO1"/>
     <mergeCell ref="AJ10:AO10"/>
-    <mergeCell ref="BE1:BJ1"/>
-    <mergeCell ref="BL1:BQ1"/>
-    <mergeCell ref="BE10:BJ10"/>
-    <mergeCell ref="BL10:BQ10"/>
-    <mergeCell ref="BS1:BX1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="O1:T1"/>
-    <mergeCell ref="O10:T10"/>
-    <mergeCell ref="V1:AA1"/>
-    <mergeCell ref="V10:AA10"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="H10:M10"/>
-    <mergeCell ref="CG1:CL1"/>
-    <mergeCell ref="CN1:CS1"/>
-    <mergeCell ref="BS10:BX10"/>
-    <mergeCell ref="BZ10:CE10"/>
-    <mergeCell ref="CG10:CL10"/>
-    <mergeCell ref="CN10:CS10"/>
-    <mergeCell ref="BZ1:CE1"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>